<commit_message>
Updated main script with enhanced logging and error handling
</commit_message>
<xml_diff>
--- a/test_results/currency_test_summary.xlsx
+++ b/test_results/currency_test_summary.xlsx
@@ -448,7 +448,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="32" customWidth="1" min="1" max="1"/>
+    <col width="72" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="40" customWidth="1" min="4" max="4"/>
@@ -479,7 +479,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/</t>
+          <t>https://www.alojamiento.io/property/mall-of-i-stanbul-3/BC-6975002/</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">

</xml_diff>